<commit_message>
Updated tests with breakpoints/screenshots
</commit_message>
<xml_diff>
--- a/Cactusforce2022/templates/TestData.xlsx
+++ b/Cactusforce2022/templates/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16156\git\Cactusforce\Cactusforce2022\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85C3FDD-1186-46FD-8D00-21F24E35719D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A97B3C8-19D3-4651-B447-985003D6BC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="24420" windowHeight="15600" xr2:uid="{8EEFB806-885C-4842-906B-A03F378F4A78}"/>
+    <workbookView xWindow="3308" yWindow="3308" windowWidth="18225" windowHeight="11332" activeTab="1" xr2:uid="{8EEFB806-885C-4842-906B-A03F378F4A78}"/>
   </bookViews>
   <sheets>
     <sheet name="Cars" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
-  <si>
-    <t>LeadName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>ExteriorColor</t>
   </si>
@@ -58,9 +55,6 @@
     <t>Black</t>
   </si>
   <si>
-    <t>Martha Bixby</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -97,7 +91,22 @@
     <t>Pink</t>
   </si>
   <si>
-    <t>Marty McFly</t>
+    <t>Martha</t>
+  </si>
+  <si>
+    <t>Bixby</t>
+  </si>
+  <si>
+    <t>martha.bixby@demo.mail</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>1-222-505-424</t>
   </si>
 </sst>
 </file>
@@ -460,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E906DD16-FE68-4C62-B068-B0412249C7FE}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -474,46 +483,37 @@
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -523,62 +523,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7D75E8-357D-40B1-BC07-4207DAE264D3}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.53125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="F3" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{60BBB28D-59A5-405C-9092-B639A5B65CA6}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{2A1C48DF-A19C-46B3-9A07-F5DCAFF782E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>